<commit_message>
update payload curve calc
</commit_message>
<xml_diff>
--- a/Payload curve calulcations.xlsx
+++ b/Payload curve calulcations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satur\Documents\Github\MAE94-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{253E587A-A918-40D8-8490-0EA8EAA294D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FC7024-8886-477A-8890-ECEC04501C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{204462A5-6728-41E2-8E4E-54A57707AC5D}"/>
   </bookViews>
@@ -127,7 +127,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -313,43 +317,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.0065165949653587</c:v>
+                  <c:v>5.625829748267952E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1447359836901116</c:v>
+                  <c:v>0.12536799184505593</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3046368451560031</c:v>
+                  <c:v>0.2053184225780017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4917548745309823</c:v>
+                  <c:v>0.29887743726549143</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7136855605338643</c:v>
+                  <c:v>0.40984278026693199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9811404898193892</c:v>
+                  <c:v>0.54357024490969452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3097279743701757</c:v>
+                  <c:v>0.70786398718508814</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7231122291276071</c:v>
+                  <c:v>0.91455611456380337</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2589807075168795</c:v>
+                  <c:v>1.1824903537584399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9812382218676374</c:v>
+                  <c:v>1.5436191109338193</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0076041633134514</c:v>
+                  <c:v>2.0568020816567261</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.5813652735303627</c:v>
+                  <c:v>2.8436826367651813</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.2996799184504688</c:v>
+                  <c:v>4.2028399592252343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1254,8 +1258,8 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CE43A6E6-9552-4752-AA96-20FB760F7988}" name="Max length (m)" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{209F3E71-343F-4275-8BB4-88EEF5CC7548}" name="Payload (kg)"/>
-    <tableColumn id="3" xr3:uid="{CF173705-9066-4C59-8B5B-5B47846B803E}" name="Shaft Torque (Nm)" totalsRowFunction="sum">
-      <calculatedColumnFormula>((B5/2)*($B$3+$C5)*9.81)/5</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{CF173705-9066-4C59-8B5B-5B47846B803E}" name="Shaft Torque (Nm)" totalsRowFunction="sum" dataDxfId="0">
+      <calculatedColumnFormula>((B5)*($B$3+$C5)*9.81)/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -1582,7 +1586,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,14 +1638,14 @@
         <v>0.59</v>
       </c>
       <c r="C5">
-        <v>1.0065165949653587</v>
+        <v>5.625829748267952E-2</v>
       </c>
       <c r="D5">
-        <f>((B5/2)*($B$3+$C5)*9.81)/5</f>
+        <f t="shared" ref="D5:D17" si="0">((B5)*($B$3+$C5)*9.81)/5</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="F5">
-        <f>((B5/2)*($B$3+$C5)*9.81)/5</f>
+        <f>((B5)*($B$3+$C5)*9.81)/5</f>
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1650,15 +1654,15 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C6">
-        <v>1.1447359836901116</v>
+        <v>0.12536799184505593</v>
       </c>
       <c r="D6">
-        <f>((B6/2)*($B$3+$C6)*9.81)/5</f>
-        <v>1.0999999999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F17" si="0">((B6/2)*($B$3+$C6)*9.81)/5</f>
-        <v>1.0999999999999999</v>
+        <f t="shared" ref="F6:F17" si="1">((B6)*($B$3+$C6)*9.81)/5</f>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1666,15 +1670,15 @@
         <v>0.51</v>
       </c>
       <c r="C7">
-        <v>1.3046368451560031</v>
+        <v>0.2053184225780017</v>
       </c>
       <c r="D7">
-        <f>((B7/2)*($B$3+$C7)*9.81)/5</f>
-        <v>1.0999999999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1682,15 +1686,15 @@
         <v>0.47</v>
       </c>
       <c r="C8">
-        <v>1.4917548745309823</v>
+        <v>0.29887743726549143</v>
       </c>
       <c r="D8">
-        <f>((B8/2)*($B$3+$C8)*9.81)/5</f>
-        <v>1.0999999999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000003</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1698,15 +1702,15 @@
         <v>0.43</v>
       </c>
       <c r="C9">
-        <v>1.7136855605338643</v>
+        <v>0.40984278026693199</v>
       </c>
       <c r="D9">
-        <f>((B9/2)*($B$3+$C9)*9.81)/5</f>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="1"/>
+        <v>1.0999999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1714,14 +1718,14 @@
         <v>0.39</v>
       </c>
       <c r="C10">
-        <v>1.9811404898193892</v>
+        <v>0.54357024490969452</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:D17" si="1">((B10/2)*($B$3+$C10)*9.81)/5</f>
+        <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1730,15 +1734,15 @@
         <v>0.35</v>
       </c>
       <c r="C11">
-        <v>2.3097279743701757</v>
+        <v>0.70786398718508814</v>
       </c>
       <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="1"/>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1746,15 +1750,15 @@
         <v>0.310000000000001</v>
       </c>
       <c r="C12">
-        <v>2.7231122291276071</v>
+        <v>0.91455611456380337</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="1"/>
-        <v>1.1000000000000003</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000003</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,15 +1766,15 @@
         <v>0.27000000000000102</v>
       </c>
       <c r="C13">
-        <v>3.2589807075168795</v>
+        <v>1.1824903537584399</v>
       </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000003</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>1.1000000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,15 +1782,15 @@
         <v>0.23000000000000101</v>
       </c>
       <c r="C14">
-        <v>3.9812382218676374</v>
+        <v>1.5436191109338193</v>
       </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="1"/>
-        <v>1.0999999999999999</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>1.0999999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1794,15 +1798,15 @@
         <v>0.190000000000001</v>
       </c>
       <c r="C15">
-        <v>5.0076041633134514</v>
+        <v>2.0568020816567261</v>
       </c>
       <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000003</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <v>1.1000000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1810,14 +1814,14 @@
         <v>0.15000000000000099</v>
       </c>
       <c r="C16">
-        <v>6.5813652735303627</v>
+        <v>2.8436826367651813</v>
       </c>
       <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000003</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="1"/>
-        <v>1.1000000000000003</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
         <v>1.1000000000000003</v>
       </c>
     </row>
@@ -1826,14 +1830,14 @@
         <v>0.110000000000001</v>
       </c>
       <c r="C17">
-        <v>9.2996799184504688</v>
+        <v>4.2028399592252343</v>
       </c>
       <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
     </row>

</xml_diff>